<commit_message>
Updated model and files
</commit_message>
<xml_diff>
--- a/excel/financial_model.xlsx
+++ b/excel/financial_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/409575d5404c8d5e/Desktop/Projects/vscode/Payflow/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1193" documentId="8_{6FDF3AD4-82DB-4513-85A3-8D1BDB68F282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0D3AEF5-46DA-4678-9FA7-0E0700784D02}"/>
+  <xr:revisionPtr revIDLastSave="1474" documentId="8_{6FDF3AD4-82DB-4513-85A3-8D1BDB68F282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{715215E3-1F1C-4741-82F4-32BDD120C600}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="360" windowWidth="28635" windowHeight="14745" activeTab="5" xr2:uid="{F10EC9A2-7D04-433E-8D71-4CAFF0736531}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F10EC9A2-7D04-433E-8D71-4CAFF0736531}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
@@ -118,60 +118,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{C9CEA1E9-615E-49C6-8BAA-EACD8857EEBA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Grant Gamble:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Source: Q4 2024 Actuals</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{84BD209C-C4D4-46B4-9017-A2A904195F19}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Grant Gamble:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Source: Q4 2024 Actuals</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t>PAYFLOW COMMERCE - Q4 2024 FINANCIAL MODEL</t>
   </si>
@@ -221,18 +173,6 @@
     <t>Total OpEx %</t>
   </si>
   <si>
-    <t>Fraud Assumptions</t>
-  </si>
-  <si>
-    <t>Current Fraud Rate (Q4 2024)</t>
-  </si>
-  <si>
-    <t>Fraud Loss (Q4 2024)</t>
-  </si>
-  <si>
-    <t>Fraud Rate (with controls - Q1 2025)</t>
-  </si>
-  <si>
     <t>Q1 2025 Forecast</t>
   </si>
   <si>
@@ -320,12 +260,6 @@
     <t>KEY INSIGHTS:</t>
   </si>
   <si>
-    <t>• Revenue exceeded budget due to Black Friday surge</t>
-  </si>
-  <si>
-    <t>• Operating margin maintained at 7%</t>
-  </si>
-  <si>
     <t>Forecast Assumptions</t>
   </si>
   <si>
@@ -347,9 +281,6 @@
     <t>New Fraud Rate (with controls)</t>
   </si>
   <si>
-    <t>Q1 2025 FORECAST</t>
-  </si>
-  <si>
     <t>COGS (70%)</t>
   </si>
   <si>
@@ -479,7 +410,55 @@
     <t>Q4 24 Net Income</t>
   </si>
   <si>
-    <t>• Fraud losses 4.1x above budget - requires action</t>
+    <t>Target Fraud Rate (Q1)</t>
+  </si>
+  <si>
+    <t>Fraud Metrics</t>
+  </si>
+  <si>
+    <t>Actual Fraud Rate (Q4 2024)</t>
+  </si>
+  <si>
+    <t>Depreciation &amp; Amortization</t>
+  </si>
+  <si>
+    <t>Fraud losses came in below budget - fraud prevention systems effective</t>
+  </si>
+  <si>
+    <t>Net income $62K above budget (+20.4% favorable variance)</t>
+  </si>
+  <si>
+    <t>Fraud Rate %</t>
+  </si>
+  <si>
+    <t>Expected Improvement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2025 PROJECTED INCOME STATEMENT </t>
+  </si>
+  <si>
+    <t>KEY TAKEAWAYS:</t>
+  </si>
+  <si>
+    <t>Q1 revenue projected at $7.48M (6% sequential growth)</t>
+  </si>
+  <si>
+    <t>Improved fraud controls expected to reduce fraud rate from 1.83% to 1.5%</t>
+  </si>
+  <si>
+    <t>Net margin forecast to improve to 5.5% (up from 5.2% in Q4)</t>
+  </si>
+  <si>
+    <t>Operating leverage driving margin expansion despite modest revenue growth</t>
+  </si>
+  <si>
+    <t>Operating income beat budget by 16.4% ($70K favorable variance)</t>
+  </si>
+  <si>
+    <t>Gross profit increased proportionally (+16.4% or $299K)</t>
+  </si>
+  <si>
+    <t>Revenue exceeded budget by 16.4% ($997K) due to strong December sales</t>
   </si>
 </sst>
 </file>
@@ -493,7 +472,7 @@
     <numFmt numFmtId="167" formatCode="0.0%;\(0.0%\);\-"/>
     <numFmt numFmtId="168" formatCode="0.00%;\(0.00%\);\-"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,8 +623,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -693,10 +685,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -707,8 +700,6 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -736,18 +727,40 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1102,11 +1115,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCE6E0D-83E0-4EFB-B76A-DF5781771D29}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,54 +1249,52 @@
         <v>0.23</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="37">
+        <v>1.83E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="10">
-        <v>7.0300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="6">
-        <v>496406</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="34">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="34">
+        <v>17</v>
+      </c>
+      <c r="B32" s="31">
         <v>0.06</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="6">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6">
         <v>7480000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="35">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1294,13 +1305,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714D8FD8-2E34-4EE4-BB13-3D00AAC2ED0F}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,161 +1322,161 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>26</v>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>31</v>
+      <c r="A3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="16">
+        <v>28</v>
+      </c>
+      <c r="B5" s="14">
         <f>Assumptions!B8</f>
         <v>1954516</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <f>Assumptions!B9</f>
         <v>2379298</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <f>Assumptions!B10</f>
         <v>2722787</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <f>SUM(B5:D5)</f>
         <v>7056601</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="16">
+        <v>29</v>
+      </c>
+      <c r="B6" s="14">
         <f>B5*Assumptions!$B$15</f>
         <v>1368161.2</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="14">
         <f>C5*Assumptions!$B$15</f>
         <v>1665508.5999999999</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="14">
         <f>D5*Assumptions!$B$15</f>
         <v>1905950.9</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="15">
         <f>SUM(B6:D6)</f>
         <v>4939620.6999999993</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="18">
+        <v>30</v>
+      </c>
+      <c r="B7" s="16">
         <f>B5-B6</f>
         <v>586354.80000000005</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <f>C5-C6</f>
         <v>713789.40000000014</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <f>D5-D6</f>
         <v>816836.10000000009</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f>SUM(B7:D7)</f>
         <v>2116980.3000000003</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <f>B7/B5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <f>C7/C5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <f>D7/D5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f>E7/E5</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <f>B5*Assumptions!$B$20</f>
         <v>195451.6</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <f>C5*Assumptions!$B$20</f>
         <v>237929.80000000002</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <f>D5*Assumptions!$B$20</f>
         <v>272278.7</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="15">
         <f>SUM(B11:D11)</f>
         <v>705660.10000000009</v>
       </c>
@@ -1474,19 +1485,19 @@
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <f>B5*Assumptions!$B$21</f>
         <v>39090.32</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <f>C5*Assumptions!$B$21</f>
         <v>47585.96</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="14">
         <f>D5*Assumptions!$B$21</f>
         <v>54455.74</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="15">
         <f>SUM(B12:D12)</f>
         <v>141132.01999999999</v>
       </c>
@@ -1495,19 +1506,19 @@
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <f>B5*Assumptions!$B$22</f>
         <v>97725.8</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <f>C5*Assumptions!$B$22</f>
         <v>118964.90000000001</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="14">
         <f>D5*Assumptions!$B$22</f>
         <v>136139.35</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="15">
         <f>SUM(B13:D13)</f>
         <v>352830.05000000005</v>
       </c>
@@ -1516,147 +1527,161 @@
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <f>B5*Assumptions!$B$23</f>
         <v>117270.95999999999</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <f>C5*Assumptions!$B$23</f>
         <v>142757.88</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="14">
         <f>D5*Assumptions!$B$23</f>
         <v>163367.22</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="15">
         <f>SUM(B14:D14)</f>
         <v>423396.06</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="18">
+        <v>32</v>
+      </c>
+      <c r="B15" s="16">
         <f>SUM(B11:B14)</f>
         <v>449538.68000000005</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="16">
         <f>SUM(C11:C14)</f>
         <v>547238.54</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <f>SUM(D11:D14)</f>
         <v>626241.01</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <f>SUM(B15:D15)</f>
         <v>1623018.23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="18">
+        <v>33</v>
+      </c>
+      <c r="B17" s="16">
         <f>B7-B15</f>
         <v>136816.12</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="16">
         <f>C7-C15</f>
         <v>166550.8600000001</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <f>D7-D15</f>
         <v>190595.09000000008</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <f>SUM(B17:D17)</f>
         <v>493962.07000000018</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="20">
+      <c r="A18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="18">
         <f>B17/B5</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="18">
         <f>C17/C5</f>
         <v>7.0000000000000048E-2</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="18">
         <f>D17/D5</f>
         <v>7.0000000000000034E-2</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <f>E17/E5</f>
         <v>7.0000000000000021E-2</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="16">
-        <f>B5*Assumptions!$B$29</f>
-        <v>137402.4748</v>
-      </c>
-      <c r="C20" s="16">
-        <f>C5*Assumptions!$B$29</f>
-        <v>167264.64939999999</v>
-      </c>
-      <c r="D20" s="16">
-        <f>D5*Assumptions!$B$29</f>
-        <v>191411.92610000001</v>
-      </c>
-      <c r="E20" s="17">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="14">
+        <f>B5*Assumptions!$B$28</f>
+        <v>35767.642800000001</v>
+      </c>
+      <c r="C20" s="14">
+        <f>C5*Assumptions!$B$28</f>
+        <v>43541.153400000003</v>
+      </c>
+      <c r="D20" s="14">
+        <f>D5*Assumptions!$B$28</f>
+        <v>49827.002099999998</v>
+      </c>
+      <c r="E20" s="15">
         <f>SUM(B20:D20)</f>
-        <v>496079.0503</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="21">
+        <v>129135.79830000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="19">
         <f>B17-B20</f>
-        <v>-586.35480000000098</v>
-      </c>
-      <c r="C21" s="21">
+        <v>101048.47719999999</v>
+      </c>
+      <c r="C22" s="19">
         <f>C17-C20</f>
-        <v>-713.78939999989234</v>
-      </c>
-      <c r="D21" s="21">
+        <v>123009.70660000009</v>
+      </c>
+      <c r="D22" s="19">
         <f>D17-D20</f>
-        <v>-816.83609999992768</v>
-      </c>
-      <c r="E21" s="21">
-        <f>SUM(B21:D21)</f>
-        <v>-2116.980299999821</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="20">
-        <f>B21/B5</f>
-        <v>-3.0000000000000052E-4</v>
-      </c>
-      <c r="C22" s="20">
-        <f>C21/C5</f>
-        <v>-2.9999999999995476E-4</v>
-      </c>
-      <c r="D22" s="20">
-        <f>D21/D5</f>
-        <v>-2.9999999999997346E-4</v>
-      </c>
-      <c r="E22" s="20">
-        <f>E21/E5</f>
-        <v>-2.9999999999997466E-4</v>
+        <v>140768.0879000001</v>
+      </c>
+      <c r="E22" s="19">
+        <f>SUM(B22:D22)</f>
+        <v>364826.27170000016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="18">
+        <f>B22/B5</f>
+        <v>5.1699999999999996E-2</v>
+      </c>
+      <c r="C23" s="18">
+        <f>C22/C5</f>
+        <v>5.1700000000000038E-2</v>
+      </c>
+      <c r="D23" s="18">
+        <f>D22/D5</f>
+        <v>5.1700000000000038E-2</v>
+      </c>
+      <c r="E23" s="18">
+        <f>E22/E5</f>
+        <v>5.1700000000000024E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1668,9 +1693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51536A83-FB50-4363-B882-483F78DE5EFF}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,148 +1706,148 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>30</v>
+      <c r="A2" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="32">
-        <f>'Cash Flow'!B25</f>
-        <v>782883.01970000018</v>
+        <v>59</v>
+      </c>
+      <c r="B6" s="30">
+        <f>'Cash Flow'!B26</f>
+        <v>1264826.2717000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="23">
+        <v>60</v>
+      </c>
+      <c r="B7" s="21">
         <v>450000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="23">
+        <v>61</v>
+      </c>
+      <c r="B8" s="21">
         <v>200000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="18">
+        <v>62</v>
+      </c>
+      <c r="B9" s="16">
         <f>SUM(B6:B8)</f>
-        <v>1432883.0197000001</v>
+        <v>1914826.2717000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="23">
+        <v>63</v>
+      </c>
+      <c r="B11" s="21">
         <v>300000</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="27">
+        <v>64</v>
+      </c>
+      <c r="B12" s="25">
         <f>B9+B11</f>
-        <v>1732883.0197000001</v>
+        <v>2214826.2717000004</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="23">
+        <v>66</v>
+      </c>
+      <c r="B16" s="21">
         <v>350000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="23">
+        <v>67</v>
+      </c>
+      <c r="B17" s="21">
         <v>150000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="18">
+        <v>68</v>
+      </c>
+      <c r="B18" s="16">
         <f>SUM(B16:B17)</f>
         <v>500000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="23">
+        <v>70</v>
+      </c>
+      <c r="B22" s="21">
         <v>1000000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="17">
+        <v>73</v>
+      </c>
+      <c r="B23" s="15">
         <f>B12-B18-B22-B24</f>
-        <v>234999.99999999988</v>
+        <v>350000.00000000023</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="28">
-        <f>'Income Statement'!E21</f>
-        <v>-2116.980299999821</v>
+        <v>74</v>
+      </c>
+      <c r="B24" s="26">
+        <f>'Income Statement'!E22</f>
+        <v>364826.27170000016</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="25">
+        <v>71</v>
+      </c>
+      <c r="B25" s="23">
         <f>SUM(B22:B24)</f>
-        <v>1232883.0197000001</v>
+        <v>1714826.2717000004</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="27">
+        <v>72</v>
+      </c>
+      <c r="B26" s="25">
         <f>B18+B25</f>
-        <v>1732883.0197000001</v>
+        <v>2214826.2717000004</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1833,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08372818-B6FD-4E12-AFF0-A3F50383FE36}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,148 +1872,156 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>30</v>
+      <c r="A2" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="16">
-        <f>'Income Statement'!E21</f>
-        <v>-2116.980299999821</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="14">
+        <f>'Income Statement'!E22</f>
+        <v>364826.27170000016</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>84</v>
+      <c r="A8" s="33" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="23">
-        <v>-50000</v>
+      <c r="A9" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="21">
+        <v>15000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="23">
-        <v>-30000</v>
+        <v>78</v>
+      </c>
+      <c r="B10" s="21">
+        <v>-50000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="23">
-        <v>40000</v>
+        <v>79</v>
+      </c>
+      <c r="B11" s="21">
+        <v>-30000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="21">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="21">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="23">
+        <f>SUM(B6:B13)</f>
+        <v>364826.27170000016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="21">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="23">
+        <f>B17</f>
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="23">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="25">
-        <f>SUM(B6:B12)</f>
-        <v>-17116.980299999821</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B22">
+        <f>B21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B24" s="28">
+        <f>B14+B18+B22</f>
+        <v>264826.27170000016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="23">
-        <v>-100000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B25" s="21">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="25">
-        <f>B16</f>
-        <v>-100000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21">
-        <f>B20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="30">
-        <f>B13+B17+B21</f>
-        <v>-117116.98029999982</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="23">
-        <v>900000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="31">
-        <f>B23+B24</f>
-        <v>782883.01970000018</v>
+      <c r="B26" s="29">
+        <f>B24+B25</f>
+        <v>1264826.2717000002</v>
       </c>
     </row>
   </sheetData>
@@ -1999,173 +2032,291 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB505A2-9FEB-43E4-A3FF-5D9FF24C4536}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="23">
+        <v>28</v>
+      </c>
+      <c r="B5" s="21">
         <v>6060000</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <f>'Income Statement'!E5</f>
         <v>7056601</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <f>C5-B5</f>
         <v>996601</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <f>D5/B5</f>
         <v>0.16445561056105609</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="23">
+      <c r="A6" s="5"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="21">
         <v>1818000</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C7" s="14">
         <f>'Income Statement'!E7</f>
         <v>2116980.3000000003</v>
       </c>
-      <c r="D6" s="17">
-        <f>C6-B6</f>
+      <c r="D7" s="15">
+        <f>C7-B7</f>
         <v>298980.30000000028</v>
       </c>
-      <c r="E6" s="20">
-        <f>D6/B6</f>
+      <c r="E7" s="18">
+        <f>D7/B7</f>
         <v>0.16445561056105626</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="23">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="42">
+        <f>'Income Statement'!E8</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D8" s="43">
+        <f>C8-B8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="43">
+        <f>D8/B8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="21">
         <v>424200</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C10" s="14">
         <f>'Income Statement'!E17</f>
         <v>493962.07000000018</v>
       </c>
-      <c r="D7" s="17">
-        <f>C7-B7</f>
+      <c r="D10" s="15">
+        <f>C10-B10</f>
         <v>69762.070000000182</v>
       </c>
-      <c r="E7" s="20">
-        <f>D7/B7</f>
+      <c r="E10" s="18">
+        <f>D10/B10</f>
         <v>0.16445561056105654</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="23">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11" s="40">
+        <f>'Income Statement'!E18</f>
+        <v>7.0000000000000021E-2</v>
+      </c>
+      <c r="D11" s="41">
+        <f>C11-B11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="41">
+        <f>D11/B11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="21">
         <v>-121200</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C13" s="14">
         <f>-'Income Statement'!E20</f>
-        <v>-496079.0503</v>
-      </c>
-      <c r="D8" s="17">
-        <f>C8-B8</f>
-        <v>-374879.0503</v>
-      </c>
-      <c r="E8" s="20">
-        <f>D8/B8</f>
-        <v>3.093061471122112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="23">
+        <v>-129135.79830000001</v>
+      </c>
+      <c r="D13" s="15">
+        <f>C13-B13</f>
+        <v>-7935.7983000000095</v>
+      </c>
+      <c r="E13" s="18">
+        <f>D13/B13</f>
+        <v>6.5476883663366417E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="C14" s="44">
+        <f>ABS(C13/C5)</f>
+        <v>1.83E-2</v>
+      </c>
+      <c r="D14" s="46">
+        <f>C14-B14</f>
+        <v>-1.7000000000000001E-3</v>
+      </c>
+      <c r="E14" s="18">
+        <f>D14/B14</f>
+        <v>-8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="21">
         <v>303000</v>
       </c>
-      <c r="C9" s="16">
-        <f>'Income Statement'!E21</f>
-        <v>-2116.980299999821</v>
-      </c>
-      <c r="D9" s="17">
-        <f>C9-B9</f>
-        <v>-305116.98029999982</v>
-      </c>
-      <c r="E9" s="20">
-        <f>D9/B9</f>
-        <v>-1.0069867336633658</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>50</v>
+      <c r="C16" s="14">
+        <f>'Income Statement'!E22</f>
+        <v>364826.27170000016</v>
+      </c>
+      <c r="D16" s="15">
+        <f>C16-B16</f>
+        <v>61826.271700000158</v>
+      </c>
+      <c r="E16" s="18">
+        <f>D16/B16</f>
+        <v>0.20404710132013254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="40">
+        <f>'Income Statement'!E23</f>
+        <v>5.1700000000000024E-2</v>
+      </c>
+      <c r="D17" s="41">
+        <f>C17-B17</f>
+        <v>1.7000000000000209E-3</v>
+      </c>
+      <c r="E17" s="47">
+        <f>D17/B17</f>
+        <v>3.4000000000000419E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2175,33 +2326,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACAB08B-55FE-411D-B78C-E70EFFC243E1}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
-        <f>REPT("=",60)</f>
-        <v>============================================================</v>
+        <f>REPT("=",72)</f>
+        <v>========================================================================</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,152 +2362,230 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="16">
+        <v>47</v>
+      </c>
+      <c r="B6" s="14">
         <f>'Income Statement'!E5</f>
         <v>7056601</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="24">
-        <f>Assumptions!B38</f>
+        <v>48</v>
+      </c>
+      <c r="B7" s="22">
+        <f>Assumptions!B32</f>
         <v>0.06</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="25">
+        <v>49</v>
+      </c>
+      <c r="B8" s="23">
         <f>B6*(1+B7)</f>
         <v>7479997.0600000005</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="26">
-        <f>Assumptions!B29</f>
-        <v>7.0300000000000001E-2</v>
+        <v>50</v>
+      </c>
+      <c r="B10" s="24">
+        <f>Assumptions!B28</f>
+        <v>1.83E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="35">
-        <f>Assumptions!B32</f>
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="17">
+        <v>51</v>
+      </c>
+      <c r="B11" s="32">
+        <f>Assumptions!B34</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="49">
+        <f>B10-B11</f>
+        <v>3.3000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="15">
         <f>B8</f>
         <v>7479997.0600000005</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="17">
-        <f>B15*0.7</f>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="15">
+        <f>B16*0.7</f>
         <v>5235997.9419999998</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="16">
+        <f>B16-B17</f>
+        <v>2243999.1180000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="52">
+        <f>B18/B16</f>
+        <v>0.3000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="15">
+        <f>B16*0.23</f>
+        <v>1720399.3238000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="15">
+        <f>B18-B21</f>
+        <v>523599.79420000059</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="18">
-        <f>B15-B16</f>
-        <v>2243999.1180000007</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="17">
-        <f>B15*0.23</f>
-        <v>1720399.3238000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="17">
-        <f>B15*B11</f>
-        <v>97239.961779999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="21">
-        <f>B17-B19-B20</f>
-        <v>426359.83242000057</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="33">
-        <f>B21/B15</f>
-        <v>5.7000000000000071E-2</v>
+      <c r="B23" s="51">
+        <f>B22/B16</f>
+        <v>7.0000000000000076E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>62</v>
+      <c r="A24" s="4"/>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="15">
+        <f>B16*B11</f>
+        <v>112199.9559</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="16">
-        <f>'Income Statement'!E21</f>
-        <v>-2116.980299999821</v>
+      <c r="B26" s="50">
+        <f>B25/B16</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="17">
-        <f>B21</f>
-        <v>426359.83242000057</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="18">
-        <f>B27-B26</f>
-        <v>428476.81272000039</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="20"/>
+        <v>36</v>
+      </c>
+      <c r="B28" s="19">
+        <f>B18-B21-B25</f>
+        <v>411399.83830000059</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="50">
+        <f>B28/B16</f>
+        <v>5.5000000000000077E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="14">
+        <f>'Income Statement'!E22</f>
+        <v>364826.27170000016</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="15">
+        <f>B28</f>
+        <v>411399.83830000059</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="29">
+        <f>B34-B33</f>
+        <v>46573.566600000428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="18"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revision to multiple files
</commit_message>
<xml_diff>
--- a/excel/financial_model.xlsx
+++ b/excel/financial_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/409575d5404c8d5e/Desktop/Projects/vscode/Payflow/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1474" documentId="8_{6FDF3AD4-82DB-4513-85A3-8D1BDB68F282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{715215E3-1F1C-4741-82F4-32BDD120C600}"/>
+  <xr:revisionPtr revIDLastSave="1525" documentId="8_{6FDF3AD4-82DB-4513-85A3-8D1BDB68F282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59C845F0-7BFC-4FC2-AB2E-FE29ABEBFDA9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F10EC9A2-7D04-433E-8D71-4CAFF0736531}"/>
+    <workbookView xWindow="135" yWindow="240" windowWidth="28635" windowHeight="14745" activeTab="5" xr2:uid="{F10EC9A2-7D04-433E-8D71-4CAFF0736531}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
@@ -741,14 +741,14 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,7 +1093,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="1" width="350" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1117,14 +1117,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCE6E0D-83E0-4EFB-B76A-DF5781771D29}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1135,8 +1135,8 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
-        <f>REPT("=",80)</f>
-        <v>================================================================================</v>
+        <f>REPT("=",75)</f>
+        <v>===========================================================================</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,19 +1438,19 @@
       <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="46">
         <f>B7/B5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="46">
         <f>C7/C5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="46">
         <f>D7/D5</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="46">
         <f>E7/E5</f>
         <v>0.30000000000000004</v>
       </c>
@@ -1590,19 +1590,19 @@
       <c r="A18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="46">
         <f>B17/B5</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="46">
         <f>C17/C5</f>
         <v>7.0000000000000048E-2</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="46">
         <f>D17/D5</f>
         <v>7.0000000000000034E-2</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="46">
         <f>E17/E5</f>
         <v>7.0000000000000021E-2</v>
       </c>
@@ -1667,19 +1667,19 @@
       <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="46">
         <f>B22/B5</f>
         <v>5.1699999999999996E-2</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="46">
         <f>C22/C5</f>
         <v>5.1700000000000038E-2</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="46">
         <f>D22/D5</f>
         <v>5.1700000000000038E-2</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="46">
         <f>E22/E5</f>
         <v>5.1700000000000024E-2</v>
       </c>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51536A83-FB50-4363-B882-483F78DE5EFF}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -2038,7 +2038,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,18 +2226,18 @@
       <c r="A14" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="51">
         <v>0.02</v>
       </c>
       <c r="C14" s="44">
         <f>ABS(C13/C5)</f>
         <v>1.83E-2</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <f>C14-B14</f>
         <v>-1.7000000000000001E-3</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="46">
         <f>D14/B14</f>
         <v>-8.5000000000000006E-2</v>
       </c>
@@ -2273,18 +2273,18 @@
       <c r="A17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="51">
         <v>0.05</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="44">
         <f>'Income Statement'!E23</f>
         <v>5.1700000000000024E-2</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="45">
         <f>C17-B17</f>
         <v>1.7000000000000209E-3</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="52">
         <f>D17/B17</f>
         <v>3.4000000000000419E-2</v>
       </c>
@@ -2328,14 +2328,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACAB08B-55FE-411D-B78C-E70EFFC243E1}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2409,7 +2409,7 @@
       <c r="A12" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="47">
         <f>B10-B11</f>
         <v>3.3000000000000008E-3</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="A19" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="52">
+      <c r="B19" s="50">
         <f>B18/B16</f>
         <v>0.3000000000000001</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="A23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="51">
+      <c r="B23" s="49">
         <f>B22/B16</f>
         <v>7.0000000000000076E-2</v>
       </c>
@@ -2499,7 +2499,7 @@
       <c r="A26" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="50">
+      <c r="B26" s="48">
         <f>B25/B16</f>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -2521,7 +2521,7 @@
       <c r="A29" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="50">
+      <c r="B29" s="48">
         <f>B28/B16</f>
         <v>5.5000000000000077E-2</v>
       </c>

</xml_diff>